<commit_message>
v1.1.6 with new spectra for the analytical model
</commit_message>
<xml_diff>
--- a/tdcrpy/validation/validationCo-60_v2.xlsx
+++ b/tdcrpy/validation/validationCo-60_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python_modules\TDCRPy\TDCRPy\tdcrpy\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D076390-83EC-44D2-B88C-14F6B4AD4140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D240CE3-3A39-4C0B-AC4C-25BC5DEB3B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="264" yWindow="5544" windowWidth="18552" windowHeight="6684" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="71">
   <si>
     <t>Reference Co-60 (NIST)</t>
   </si>
@@ -249,6 +249,9 @@
   <si>
     <t>conv</t>
   </si>
+  <si>
+    <t>Version 1.1.6</t>
+  </si>
 </sst>
 </file>
 
@@ -394,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -429,15 +432,13 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="71">
     <dxf>
       <numFmt numFmtId="168" formatCode="0.0"/>
       <fill>
@@ -446,6 +447,51 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="0.0"/>
@@ -473,6 +519,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2160,7 +2215,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tables!$N$130</c15:sqref>
@@ -2180,7 +2235,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tables!$A$131:$A$154</c15:sqref>
@@ -2267,7 +2322,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tables!$N$131:$N$154</c15:sqref>
@@ -2353,7 +2408,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-E7DA-483B-8340-7FCBF7C44900}"/>
                   </c:ext>
@@ -2382,7 +2437,7 @@
                   <c:noEndCap val="0"/>
                   <c:plus>
                     <c:numRef>
-                      <c:extLst>
+                      <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                         <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                           <c15:formulaRef>
                             <c15:sqref>Tables!$C$86:$C$98</c15:sqref>
@@ -2436,7 +2491,7 @@
                   </c:plus>
                   <c:minus>
                     <c:numRef>
-                      <c:extLst>
+                      <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                         <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                           <c15:formulaRef>
                             <c15:sqref>Tables!$C$86:$C$98</c15:sqref>
@@ -2639,7 +2694,7 @@
                   <c:noEndCap val="0"/>
                   <c:plus>
                     <c:numRef>
-                      <c:extLst>
+                      <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                         <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                           <c15:formulaRef>
                             <c15:sqref>Tables!$C$108:$C$120</c15:sqref>
@@ -2690,7 +2745,7 @@
                   </c:plus>
                   <c:minus>
                     <c:numRef>
-                      <c:extLst>
+                      <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                         <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                           <c15:formulaRef>
                             <c15:sqref>Tables!$C$108:$C$120</c15:sqref>
@@ -8287,7 +8342,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F388A5FC-AE15-4458-B3E9-16AF6815805A}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="36" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8298,7 +8353,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{18989E30-B0EA-429F-B87A-6F4A60F8F2EB}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="95" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="36" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8309,7 +8364,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9288379" cy="6063916"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8342,7 +8397,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9288379" cy="6063916"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8493,30 +8548,60 @@
   <autoFilter ref="A14:I31" xr:uid="{CE154909-7646-477D-8B60-509F398D009F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DDAABB74-83B7-4A9A-A978-ACBC6E410C19}" name="N"/>
-    <tableColumn id="2" xr3:uid="{0AA70936-8F84-45A0-BDA6-0B48F50D8456}" name="eff (stochastic)" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{CC8B2236-DD4D-4D4A-B450-AF4A42700DB8}" name="u(eff)" dataDxfId="55" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{0AA70936-8F84-45A0-BDA6-0B48F50D8456}" name="eff (stochastic)" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{CC8B2236-DD4D-4D4A-B450-AF4A42700DB8}" name="u(eff)" dataDxfId="69" dataCellStyle="Percent"/>
     <tableColumn id="3" xr3:uid="{F519117B-BD8C-4D86-8925-34E52A9B33AA}" name="time /s"/>
-    <tableColumn id="4" xr3:uid="{4C05EF6D-660F-41D6-BD8A-A706F835288E}" name="error" dataDxfId="54" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{4C05EF6D-660F-41D6-BD8A-A706F835288E}" name="error" dataDxfId="68" dataCellStyle="Percent">
       <calculatedColumnFormula>B15/B$5-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C52CC8CE-0CF9-4BDD-85DA-B7B7E424ADFB}" name="L /keV-1" dataDxfId="53" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{FF4F8F5D-D5E2-4E8C-95FD-6BDE1A995214}" name="LA /keV-1" dataDxfId="52" dataCellStyle="Percent"/>
-    <tableColumn id="8" xr3:uid="{AD370BAA-110E-45FB-8017-6C63B1F0C6DC}" name="LB /keV-1" dataDxfId="51" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{0D9EDC29-DB17-43EE-9A9E-873BA5DEC89A}" name="LC /keV-1" dataDxfId="50" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{C52CC8CE-0CF9-4BDD-85DA-B7B7E424ADFB}" name="L /keV-1" dataDxfId="67" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{FF4F8F5D-D5E2-4E8C-95FD-6BDE1A995214}" name="LA /keV-1" dataDxfId="66" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{AD370BAA-110E-45FB-8017-6C63B1F0C6DC}" name="LB /keV-1" dataDxfId="65" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{0D9EDC29-DB17-43EE-9A9E-873BA5DEC89A}" name="LC /keV-1" dataDxfId="64" dataCellStyle="Percent"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{78223100-27A6-46D3-9F45-28E2D0C102E0}" name="Table47912" displayName="Table47912" ref="A228:M251" totalsRowShown="0">
+  <autoFilter ref="A228:M251" xr:uid="{78223100-27A6-46D3-9F45-28E2D0C102E0}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{45FA29F9-7193-43B7-A1F5-19D385ED8402}" name="N"/>
+    <tableColumn id="2" xr3:uid="{DAAF6AD1-38AB-4EF8-96AC-F728FFC5D112}" name="eff (stochastic)" dataDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{76970522-5EED-44C5-8AEE-275C57FE2786}" name="std" dataDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{37E30C36-6877-4C75-A32C-8883F5BB106F}" name="time /s"/>
+    <tableColumn id="9" xr3:uid="{604AB221-91DC-4D68-B1E0-A7407FD493AB}" name="interation" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{38D53FAD-6F5C-4CF5-B95A-3D60E65BC1B8}" name="error" dataDxfId="3">
+      <calculatedColumnFormula>B229/B$5-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{9A9FA1C5-E36C-4C9F-A102-08E93FA78A66}" name="L /keV-1"/>
+    <tableColumn id="13" xr3:uid="{32ED1515-757B-4B11-8DAC-D9A2210702DC}" name="LA /keV-1"/>
+    <tableColumn id="12" xr3:uid="{9D36FEA7-0704-44F1-85BC-2248BA9A0657}" name="LB /keV-1"/>
+    <tableColumn id="11" xr3:uid="{E5A77F2A-B3C4-4422-92E1-7A19B202B4D7}" name="LC /keV-1"/>
+    <tableColumn id="7" xr3:uid="{CAB2DCDF-9259-4B12-BF2F-0B1C26960770}" name="speed /s" dataDxfId="2">
+      <calculatedColumnFormula>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{560AC3B3-9B23-4FE2-89D0-F2A1B551B6E4}" name="time /h" dataDxfId="1">
+      <calculatedColumnFormula>Table47912[[#This Row],[time /s]]/3600</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{A6CECFD7-C8F7-4CD3-9C8D-02D23C237D5B}" name="Z-score" dataDxfId="0">
+      <calculatedColumnFormula>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1A0E7B8-D1BC-47E5-92B3-1AE140DABEDC}" name="Table2" displayName="Table2" ref="A45:F54" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48" tableBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1A0E7B8-D1BC-47E5-92B3-1AE140DABEDC}" name="Table2" displayName="Table2" ref="A45:F54" totalsRowShown="0" headerRowDxfId="63" headerRowBorderDxfId="62" tableBorderDxfId="61">
   <autoFilter ref="A45:F54" xr:uid="{B1A0E7B8-D1BC-47E5-92B3-1AE140DABEDC}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2A7212F2-06BB-4D63-B68E-00B66F9BA6D8}" name="N"/>
-    <tableColumn id="2" xr3:uid="{D4B2378E-DEE0-403B-9A01-7D7DAF895C2A}" name="eff (stochastic)" dataDxfId="46" dataCellStyle="Percent"/>
-    <tableColumn id="9" xr3:uid="{DCBF8CA2-4B7B-45F6-A4C1-21C25175DEC1}" name="std" dataDxfId="45" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{76B9D488-065E-48FD-8C5C-DFB2F4A7C18C}" name="time /s" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{B3632296-46F8-4FFB-B621-41267E9BD825}" name="error" dataDxfId="43">
+    <tableColumn id="2" xr3:uid="{D4B2378E-DEE0-403B-9A01-7D7DAF895C2A}" name="eff (stochastic)" dataDxfId="60" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{DCBF8CA2-4B7B-45F6-A4C1-21C25175DEC1}" name="std" dataDxfId="59" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{76B9D488-065E-48FD-8C5C-DFB2F4A7C18C}" name="time /s" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{B3632296-46F8-4FFB-B621-41267E9BD825}" name="error" dataDxfId="57">
       <calculatedColumnFormula>B46/B$5-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{FC6E204E-4636-4F11-8582-10674B968FF7}" name="L /keV-1"/>
@@ -8526,21 +8611,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98A4BCFE-02B5-4530-A1DC-143F7E0EE115}" name="Table24" displayName="Table24" ref="A62:H71" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98A4BCFE-02B5-4530-A1DC-143F7E0EE115}" name="Table24" displayName="Table24" ref="A62:H71" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54">
   <autoFilter ref="A62:H71" xr:uid="{98A4BCFE-02B5-4530-A1DC-143F7E0EE115}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{8F2C12A2-FD44-4CE7-AE3E-946D17F8E77D}" name="N"/>
-    <tableColumn id="2" xr3:uid="{DFE623A6-4D03-4FC8-8636-F552CAFF9337}" name="eff (stochastic)" dataDxfId="39" dataCellStyle="Percent"/>
-    <tableColumn id="9" xr3:uid="{79B4CF1D-0184-4DC2-9C5F-BA40F6EAABC6}" name="std" dataDxfId="38" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{7F75FB14-269C-48EF-ACB6-BFCBC8D8F3E9}" name="time /s" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{5373102D-9EEB-4008-B4E8-DDFBFA8B5659}" name="error" dataDxfId="36">
+    <tableColumn id="2" xr3:uid="{DFE623A6-4D03-4FC8-8636-F552CAFF9337}" name="eff (stochastic)" dataDxfId="53" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{79B4CF1D-0184-4DC2-9C5F-BA40F6EAABC6}" name="std" dataDxfId="52" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{7F75FB14-269C-48EF-ACB6-BFCBC8D8F3E9}" name="time /s" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{5373102D-9EEB-4008-B4E8-DDFBFA8B5659}" name="error" dataDxfId="50">
       <calculatedColumnFormula>B63/B$5-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{2EA1A9A7-9F1E-4C41-8D47-473AFC686CDF}" name="L /keV-1"/>
-    <tableColumn id="6" xr3:uid="{6FA56703-B0EB-4061-BA8B-CBE48889BD88}" name="speed" dataDxfId="35">
+    <tableColumn id="6" xr3:uid="{6FA56703-B0EB-4061-BA8B-CBE48889BD88}" name="speed" dataDxfId="49">
       <calculatedColumnFormula>Table24[[#This Row],[N]]/Table24[[#This Row],[time /s]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4668A5EC-12A1-4427-BA2D-CC7DA1B9E712}" name="time/h" dataDxfId="34">
+    <tableColumn id="7" xr3:uid="{4668A5EC-12A1-4427-BA2D-CC7DA1B9E712}" name="time/h" dataDxfId="48">
       <calculatedColumnFormula>Table24[[#This Row],[time /s]]/3600</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8553,17 +8638,17 @@
   <autoFilter ref="A75:H78" xr:uid="{5754EABE-BCB3-4E1A-9DB8-2647BBDDC114}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{174981E2-18F0-4578-87C4-D60BCD6AD8B8}" name="Method"/>
-    <tableColumn id="2" xr3:uid="{4C63FD53-4E05-49BB-AE06-25A9EA64DA2A}" name="eff" dataDxfId="33" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{5F8FF70E-D2C0-49A0-8AE0-991399ADA1AA}" name="u" dataDxfId="32" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{2CB36EE8-CC8A-4E9E-A506-DCD96BBC92F2}" name="time /s" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{9D6C63CC-25B7-465E-BA81-97F393A00604}" name="error" dataDxfId="30">
+    <tableColumn id="2" xr3:uid="{4C63FD53-4E05-49BB-AE06-25A9EA64DA2A}" name="eff" dataDxfId="47" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{5F8FF70E-D2C0-49A0-8AE0-991399ADA1AA}" name="u" dataDxfId="46" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{2CB36EE8-CC8A-4E9E-A506-DCD96BBC92F2}" name="time /s" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{9D6C63CC-25B7-465E-BA81-97F393A00604}" name="error" dataDxfId="44">
       <calculatedColumnFormula>B76/B$5-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{8A97AEEF-A278-406A-9A09-82BAB22A8485}" name="L/keV-1"/>
-    <tableColumn id="7" xr3:uid="{18402C67-F13C-4B86-92DE-7941792C7C21}" name="speed" dataDxfId="29">
+    <tableColumn id="7" xr3:uid="{18402C67-F13C-4B86-92DE-7941792C7C21}" name="speed" dataDxfId="43">
       <calculatedColumnFormula>10000/Table5[[#This Row],[time /s]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC928F03-2BC6-4639-8B90-568D89035180}" name="time/h" dataDxfId="28">
+    <tableColumn id="8" xr3:uid="{AC928F03-2BC6-4639-8B90-568D89035180}" name="time/h" dataDxfId="42">
       <calculatedColumnFormula>Table5[[#This Row],[time /s]]/3600</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8576,21 +8661,21 @@
   <autoFilter ref="A85:J99" xr:uid="{02403DAC-D5F4-4847-B640-D5ABB9BC5109}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F20144C8-F0B1-443F-8ACE-7A8491A3BD44}" name="N"/>
-    <tableColumn id="2" xr3:uid="{6D4919DB-A5DF-45B0-BB6B-C4792284C9D8}" name="eff (stochastic)" dataDxfId="27" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{CA5A0DF5-F5FE-4A6F-A33C-CC982089C42E}" name="std" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{6D4919DB-A5DF-45B0-BB6B-C4792284C9D8}" name="eff (stochastic)" dataDxfId="41" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{CA5A0DF5-F5FE-4A6F-A33C-CC982089C42E}" name="std" dataDxfId="40" dataCellStyle="Percent"/>
     <tableColumn id="4" xr3:uid="{18704ADD-5A08-490C-8CA4-93F4A0C99976}" name="time /s"/>
-    <tableColumn id="9" xr3:uid="{24E1A1F8-7146-4275-9A11-ECCF568B0B0E}" name="interation" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{6B02D242-A899-4DBA-9577-367B45D4142B}" name="error" dataDxfId="24">
+    <tableColumn id="9" xr3:uid="{24E1A1F8-7146-4275-9A11-ECCF568B0B0E}" name="interation" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{6B02D242-A899-4DBA-9577-367B45D4142B}" name="error" dataDxfId="38">
       <calculatedColumnFormula>B86/B$5-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{26A8B87D-A16A-4AF0-BC8E-1B00C8A244CE}" name="L /keV-1"/>
-    <tableColumn id="7" xr3:uid="{7C23E836-A52A-498C-86AF-D0584542A557}" name="speed /s" dataDxfId="23">
+    <tableColumn id="7" xr3:uid="{7C23E836-A52A-498C-86AF-D0584542A557}" name="speed /s" dataDxfId="37">
       <calculatedColumnFormula>Table4[[#This Row],[N]]*Table4[[#This Row],[interation]]/Table4[[#This Row],[time /s]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0A312CBD-58B9-48C7-9B79-0F6F994FEA00}" name="time /h" dataDxfId="22">
+    <tableColumn id="8" xr3:uid="{0A312CBD-58B9-48C7-9B79-0F6F994FEA00}" name="time /h" dataDxfId="36">
       <calculatedColumnFormula>Table4[[#This Row],[time /s]]/3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C660F51-E374-40AD-A647-0D23A74A704A}" name="Z-score" dataDxfId="21">
+    <tableColumn id="10" xr3:uid="{0C660F51-E374-40AD-A647-0D23A74A704A}" name="Z-score" dataDxfId="35">
       <calculatedColumnFormula>ABS(Table4[[#This Row],[error]])/Table4[[#This Row],[std]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8603,24 +8688,24 @@
   <autoFilter ref="A107:M121" xr:uid="{BD8F3B19-3AF7-4026-99BD-ABC18E124E71}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{2034803E-B4B6-4901-A5F9-C484A76FD21C}" name="N"/>
-    <tableColumn id="2" xr3:uid="{AC62611A-36F0-4490-BE29-4F5C95567877}" name="eff (stochastic)" dataDxfId="20" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{8A3D8C01-2B92-4C5B-81E8-E7BF75D17D6E}" name="std" dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{AC62611A-36F0-4490-BE29-4F5C95567877}" name="eff (stochastic)" dataDxfId="34" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{8A3D8C01-2B92-4C5B-81E8-E7BF75D17D6E}" name="std" dataDxfId="33" dataCellStyle="Percent"/>
     <tableColumn id="4" xr3:uid="{F780DF52-214B-4153-B238-79C45B603F23}" name="time /s"/>
-    <tableColumn id="9" xr3:uid="{7FC33D46-B3E6-4ADA-AC9B-FDF0C695575A}" name="interation" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{51424C08-23C8-4135-A6F9-E6E1E3E9E069}" name="error" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{7FC33D46-B3E6-4ADA-AC9B-FDF0C695575A}" name="interation" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{51424C08-23C8-4135-A6F9-E6E1E3E9E069}" name="error" dataDxfId="31">
       <calculatedColumnFormula>B108/B$5-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{373866C6-6FF2-4DF9-8031-12E64AF26EE9}" name="L /keV-1"/>
     <tableColumn id="13" xr3:uid="{08D2C2DF-FD03-4D21-8243-DBD2E4E3B946}" name="LA /keV-1"/>
     <tableColumn id="12" xr3:uid="{60D36303-EAB7-40E2-8770-E17A8B5DD3AE}" name="LB /keV-1"/>
     <tableColumn id="11" xr3:uid="{FD3C92D0-B313-468F-9F2B-72309F29573B}" name="LC /keV-1"/>
-    <tableColumn id="7" xr3:uid="{013B7DB1-A952-4323-BD1D-3018A2EBCF91}" name="speed /s" dataDxfId="16">
+    <tableColumn id="7" xr3:uid="{013B7DB1-A952-4323-BD1D-3018A2EBCF91}" name="speed /s" dataDxfId="30">
       <calculatedColumnFormula>Table47[[#This Row],[N]]*Table47[[#This Row],[interation]]/Table47[[#This Row],[time /s]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2142541B-6C24-4D72-823E-46165F298113}" name="time /h" dataDxfId="15">
+    <tableColumn id="8" xr3:uid="{2142541B-6C24-4D72-823E-46165F298113}" name="time /h" dataDxfId="29">
       <calculatedColumnFormula>Table47[[#This Row],[time /s]]/3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{BF5DCFC9-8584-484D-B4FC-744740AAE63E}" name="Z-score" dataDxfId="14">
+    <tableColumn id="10" xr3:uid="{BF5DCFC9-8584-484D-B4FC-744740AAE63E}" name="Z-score" dataDxfId="28">
       <calculatedColumnFormula>ABS(Table47[[#This Row],[error]])/Table47[[#This Row],[std]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8633,21 +8718,21 @@
   <autoFilter ref="A130:J154" xr:uid="{24B6E3DF-F151-43AB-98AE-88A67DD42249}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1A312C32-9FCA-41AE-BBF3-0E1189CFB3E5}" name="N"/>
-    <tableColumn id="2" xr3:uid="{23CC626A-68F3-43FF-9384-035F3812EF42}" name="eff (stochastic)" dataDxfId="13" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{FEA266E2-E5E2-4F9E-BCAB-31B870556071}" name="std" dataDxfId="12" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{23CC626A-68F3-43FF-9384-035F3812EF42}" name="eff (stochastic)" dataDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{FEA266E2-E5E2-4F9E-BCAB-31B870556071}" name="std" dataDxfId="26" dataCellStyle="Percent"/>
     <tableColumn id="4" xr3:uid="{448CB9AD-EE87-451E-8B25-0EE71085E792}" name="time /s"/>
-    <tableColumn id="9" xr3:uid="{3D2BDB44-7407-44AF-8B6D-19C74B3EF920}" name="interation" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{CF8B6E0E-B6BC-42B6-BD79-992F016E48F9}" name="error" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{3D2BDB44-7407-44AF-8B6D-19C74B3EF920}" name="interation" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{CF8B6E0E-B6BC-42B6-BD79-992F016E48F9}" name="error" dataDxfId="24">
       <calculatedColumnFormula>B131/B$5-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{6FFE4936-878E-4317-A067-EE4AC45CE5C5}" name="L /keV-1"/>
-    <tableColumn id="7" xr3:uid="{D2FB2BFE-9112-4705-9D7B-07D340DA3BBC}" name="speed /s" dataDxfId="9">
+    <tableColumn id="7" xr3:uid="{D2FB2BFE-9112-4705-9D7B-07D340DA3BBC}" name="speed /s" dataDxfId="23">
       <calculatedColumnFormula>Table48[[#This Row],[N]]*Table48[[#This Row],[interation]]/Table48[[#This Row],[time /s]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EC225E2A-8E22-4676-B463-53E0BCD0C837}" name="time /h" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{EC225E2A-8E22-4676-B463-53E0BCD0C837}" name="time /h" dataDxfId="22">
       <calculatedColumnFormula>Table48[[#This Row],[time /s]]/3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9D985096-4123-4E85-B451-0D523A795D58}" name="Z-score" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{9D985096-4123-4E85-B451-0D523A795D58}" name="Z-score" dataDxfId="21">
       <calculatedColumnFormula>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8660,25 +8745,52 @@
   <autoFilter ref="A161:M185" xr:uid="{2EAD48A6-0370-4313-99C6-706237C08F90}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{4936D717-6A48-44A9-B3F8-AD43FF4DBAEA}" name="N"/>
-    <tableColumn id="2" xr3:uid="{05152AB6-FBEE-4D8C-8972-8AADD038EDD3}" name="eff (stochastic)" dataDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{487B6454-47C0-473F-B56B-87BC9FBD6525}" name="std" dataDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{05152AB6-FBEE-4D8C-8972-8AADD038EDD3}" name="eff (stochastic)" dataDxfId="20" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{487B6454-47C0-473F-B56B-87BC9FBD6525}" name="std" dataDxfId="19" dataCellStyle="Percent"/>
     <tableColumn id="4" xr3:uid="{B06F9C07-E7BF-4288-BED3-4C97CB606F5D}" name="time /s"/>
-    <tableColumn id="9" xr3:uid="{175C5E83-32ED-47D6-837B-81D7CEDCF30F}" name="interation" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{581325E5-812B-46FB-AB3E-4F0EF2E9D513}" name="error" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{175C5E83-32ED-47D6-837B-81D7CEDCF30F}" name="interation" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{581325E5-812B-46FB-AB3E-4F0EF2E9D513}" name="error" dataDxfId="17">
       <calculatedColumnFormula>B162/B$5-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{234C2629-0DD0-4C9F-906A-25E8843F567A}" name="L /keV-1"/>
     <tableColumn id="13" xr3:uid="{EB7613CB-4675-4100-8500-0CC47CA99624}" name="LA /keV-1"/>
     <tableColumn id="12" xr3:uid="{247FDCBC-64CE-43CD-8AC9-8259472F6D90}" name="LB /keV-1"/>
     <tableColumn id="11" xr3:uid="{BC1F7DB4-29E0-4C86-B60F-ABD31D50B674}" name="LC /keV-1"/>
-    <tableColumn id="7" xr3:uid="{2AECCDA0-2990-4A3D-80AF-B2DAC0A52A36}" name="speed /s" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{2AECCDA0-2990-4A3D-80AF-B2DAC0A52A36}" name="speed /s" dataDxfId="16">
       <calculatedColumnFormula>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{47842E90-0810-4534-9AFB-FD27204EF560}" name="time /h" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{47842E90-0810-4534-9AFB-FD27204EF560}" name="time /h" dataDxfId="15">
       <calculatedColumnFormula>Table479[[#This Row],[time /s]]/3600</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C2D7729C-B424-48AD-8D16-1C4AB2258D34}" name="Z-score" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{C2D7729C-B424-48AD-8D16-1C4AB2258D34}" name="Z-score" dataDxfId="14">
       <calculatedColumnFormula>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BFA4AC05-F008-4798-BA16-6E6B5E6F1B06}" name="Table4810" displayName="Table4810" ref="A199:J222" totalsRowShown="0">
+  <autoFilter ref="A199:J222" xr:uid="{BFA4AC05-F008-4798-BA16-6E6B5E6F1B06}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{70792504-3B62-4A4E-9A4E-561921A7B151}" name="N"/>
+    <tableColumn id="2" xr3:uid="{656063D4-AEE2-4F98-A3EC-B62963955180}" name="eff (stochastic)" dataDxfId="13" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{D6444B7F-EAD4-46F9-893A-0E950CB0A556}" name="std" dataDxfId="12" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{5DE5C07E-0F95-44AF-BFC7-19CF5F0AF257}" name="time /s"/>
+    <tableColumn id="9" xr3:uid="{0BC7E258-7448-4591-BD3D-0FB0BAA94BA5}" name="interation" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{75FA500D-7717-4566-A06E-97BB06EED6CD}" name="error" dataDxfId="7">
+      <calculatedColumnFormula>B200/B$5-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{75F858FE-A078-4D42-A783-27C2E82388D6}" name="L /keV-1"/>
+    <tableColumn id="7" xr3:uid="{0F5C4193-AE61-4DBD-BEDE-66F8A36CA71E}" name="speed /s" dataDxfId="10">
+      <calculatedColumnFormula>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{A476BBAA-4C9B-4896-A471-083FADE1DF38}" name="time /h" dataDxfId="9">
+      <calculatedColumnFormula>Table4810[[#This Row],[time /s]]/3600</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{FF9CD72C-0F4A-441D-8045-B680474B4E5D}" name="Z-score" dataDxfId="8">
+      <calculatedColumnFormula>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -8948,10 +9060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P223"/>
+  <dimension ref="A1:P284"/>
   <sheetViews>
-    <sheetView topLeftCell="E125" workbookViewId="0">
-      <selection activeCell="O131" sqref="O131:O154"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11911,7 +12023,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>5.0341666666666666E-4</v>
       </c>
-      <c r="J132" s="35">
+      <c r="J132" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-8.5012795433275418E-2</v>
       </c>
@@ -11967,7 +12079,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>1.2586872222222223E-3</v>
       </c>
-      <c r="J133" s="35">
+      <c r="J133" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>0.40788397475657451</v>
       </c>
@@ -12023,7 +12135,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>2.6086177777777777E-3</v>
       </c>
-      <c r="J134" s="35">
+      <c r="J134" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.15721149141369237</v>
       </c>
@@ -12079,7 +12191,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>4.9956925000000001E-3</v>
       </c>
-      <c r="J135" s="35">
+      <c r="J135" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>0.69380507116584633</v>
       </c>
@@ -12135,7 +12247,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>1.2660654722222222E-2</v>
       </c>
-      <c r="J136" s="35">
+      <c r="J136" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.31745452837920285</v>
       </c>
@@ -12191,7 +12303,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>2.014765638888889E-2</v>
       </c>
-      <c r="J137" s="35">
+      <c r="J137" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.49227152232374477</v>
       </c>
@@ -12247,7 +12359,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>2.5221577222222225E-2</v>
       </c>
-      <c r="J138" s="35">
+      <c r="J138" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>0.41579193839605727</v>
       </c>
@@ -12303,7 +12415,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>5.0760348055555557E-2</v>
       </c>
-      <c r="J139" s="35">
+      <c r="J139" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-1.0023536261496429</v>
       </c>
@@ -12415,7 +12527,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>0.12534785500000001</v>
       </c>
-      <c r="J141" s="35">
+      <c r="J141" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>0.98884866574488528</v>
       </c>
@@ -12471,7 +12583,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>0.18746111555555556</v>
       </c>
-      <c r="J142" s="35">
+      <c r="J142" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.4307577143054287</v>
       </c>
@@ -12527,7 +12639,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>0.21026400916666665</v>
       </c>
-      <c r="J143" s="35">
+      <c r="J143" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.90379651512169934</v>
       </c>
@@ -12583,7 +12695,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>0.23437295527777779</v>
       </c>
-      <c r="J144" s="35">
+      <c r="J144" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.45967622798172797</v>
       </c>
@@ -12639,7 +12751,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>0.25139593222222223</v>
       </c>
-      <c r="J145" s="35">
+      <c r="J145" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.57151700644579262</v>
       </c>
@@ -12681,7 +12793,7 @@
         <v>20</v>
       </c>
       <c r="F146" s="21">
-        <f>B146/B$5-1</f>
+        <f t="shared" ref="F146:F154" si="17">B146/B$5-1</f>
         <v>-2.6547865333960141E-3</v>
       </c>
       <c r="G146" s="3">
@@ -12695,7 +12807,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>0.49365145500000002</v>
       </c>
-      <c r="J146" s="35">
+      <c r="J146" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-1.585374368340924</v>
       </c>
@@ -12737,7 +12849,7 @@
         <v>20</v>
       </c>
       <c r="F147" s="21">
-        <f>B147/B$5-1</f>
+        <f t="shared" si="17"/>
         <v>-4.1284331785007566E-4</v>
       </c>
       <c r="G147" s="3">
@@ -12751,7 +12863,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>0.78354702999999992</v>
       </c>
-      <c r="J147" s="35">
+      <c r="J147" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>0.75966799964432807</v>
       </c>
@@ -12793,7 +12905,7 @@
         <v>20</v>
       </c>
       <c r="F148" s="21">
-        <f>B148/B$5-1</f>
+        <f t="shared" si="17"/>
         <v>-1.1423280325291163E-3</v>
       </c>
       <c r="G148" s="3">
@@ -12807,7 +12919,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>1.0423902350000001</v>
       </c>
-      <c r="J148" s="35">
+      <c r="J148" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.17063631515317662</v>
       </c>
@@ -12849,7 +12961,7 @@
         <v>20</v>
       </c>
       <c r="F149" s="21">
-        <f>B149/B$5-1</f>
+        <f t="shared" si="17"/>
         <v>-4.9718775639395751E-4</v>
       </c>
       <c r="G149" s="3">
@@ -12863,7 +12975,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>1.2722926205555556</v>
       </c>
-      <c r="J149" s="35">
+      <c r="J149" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>0.83405414028546743</v>
       </c>
@@ -12905,7 +13017,7 @@
         <v>20</v>
       </c>
       <c r="F150" s="21">
-        <f>B150/B$5-1</f>
+        <f t="shared" si="17"/>
         <v>-1.1918886588064836E-3</v>
       </c>
       <c r="G150" s="3">
@@ -12919,7 +13031,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>1.5769363383333332</v>
       </c>
-      <c r="J150" s="35">
+      <c r="J150" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.29210837104894666</v>
       </c>
@@ -12961,7 +13073,7 @@
         <v>20</v>
       </c>
       <c r="F151" s="21">
-        <f>B151/B$5-1</f>
+        <f t="shared" si="17"/>
         <v>-2.8493218558145461E-4</v>
       </c>
       <c r="G151" s="3">
@@ -12975,7 +13087,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>1.8277614283333332</v>
       </c>
-      <c r="J151" s="35">
+      <c r="J151" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>1.3908986116945079</v>
       </c>
@@ -13017,7 +13129,7 @@
         <v>20</v>
       </c>
       <c r="F152" s="21">
-        <f>B152/B$5-1</f>
+        <f t="shared" si="17"/>
         <v>-1.8928138990281784E-4</v>
       </c>
       <c r="G152" s="3">
@@ -13031,7 +13143,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>2.0733266908333334</v>
       </c>
-      <c r="J152" s="35">
+      <c r="J152" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>1.6740373861851947</v>
       </c>
@@ -13073,7 +13185,7 @@
         <v>20</v>
       </c>
       <c r="F153" s="21">
-        <f>B153/B$5-1</f>
+        <f t="shared" si="17"/>
         <v>-1.2737901663620876E-3</v>
       </c>
       <c r="G153" s="3">
@@ -13087,7 +13199,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>2.271757401111111</v>
       </c>
-      <c r="J153" s="35">
+      <c r="J153" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-0.52322486614179786</v>
       </c>
@@ -13129,7 +13241,7 @@
         <v>20</v>
       </c>
       <c r="F154" s="21">
-        <f>B154/B$5-1</f>
+        <f t="shared" si="17"/>
         <v>-1.8028123007353125E-3</v>
       </c>
       <c r="G154">
@@ -13143,7 +13255,7 @@
         <f>Table48[[#This Row],[time /s]]/3600</f>
         <v>2.5779005502777776</v>
       </c>
-      <c r="J154" s="35">
+      <c r="J154" s="31">
         <f>(Table48[[#This Row],[eff (stochastic)]]-$C$190)/Table48[[#This Row],[std]]</f>
         <v>-1.6893994359900339</v>
       </c>
@@ -13277,7 +13389,7 @@
         <v>20</v>
       </c>
       <c r="F162" s="9">
-        <f t="shared" ref="F162:F180" si="17">B162/B$5-1</f>
+        <f t="shared" ref="F162:F180" si="18">B162/B$5-1</f>
         <v>2.6416163810667914E-2</v>
       </c>
       <c r="G162">
@@ -13323,7 +13435,7 @@
         <v>20</v>
       </c>
       <c r="F163" s="21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.6416163797431169E-2</v>
       </c>
       <c r="G163">
@@ -13369,7 +13481,7 @@
         <v>20</v>
       </c>
       <c r="F164" s="21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.9798678225280808E-2</v>
       </c>
       <c r="G164">
@@ -13415,7 +13527,7 @@
         <v>20</v>
       </c>
       <c r="F165" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.550820886939742E-2</v>
       </c>
       <c r="G165">
@@ -13461,7 +13573,7 @@
         <v>20</v>
       </c>
       <c r="F166" s="21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-1.8848051579784197E-2</v>
       </c>
       <c r="G166">
@@ -13484,7 +13596,7 @@
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>1.5803089999999999E-2</v>
       </c>
-      <c r="M166" s="35">
+      <c r="M166" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>-1.3132780394700281</v>
       </c>
@@ -13507,7 +13619,7 @@
         <v>20</v>
       </c>
       <c r="F167" s="21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-4.154843238327488E-3</v>
       </c>
       <c r="G167">
@@ -13530,7 +13642,7 @@
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>3.6146163888888888E-2</v>
       </c>
-      <c r="M167" s="35">
+      <c r="M167" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>-0.47561306150638938</v>
       </c>
@@ -13553,7 +13665,7 @@
         <v>20</v>
       </c>
       <c r="F168" s="21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3.0199075921877316E-4</v>
       </c>
       <c r="G168">
@@ -13576,7 +13688,7 @@
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>6.3845862222222216E-2</v>
       </c>
-      <c r="M168" s="35">
+      <c r="M168" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>0.27237203483738914</v>
       </c>
@@ -13599,7 +13711,7 @@
         <v>20</v>
       </c>
       <c r="F169" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.9386923732050985E-3</v>
       </c>
       <c r="G169">
@@ -13622,7 +13734,7 @@
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>8.0781708333333327E-2</v>
       </c>
-      <c r="M169" s="35">
+      <c r="M169" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>0.96144079098925062</v>
       </c>
@@ -13645,7 +13757,7 @@
         <v>20</v>
       </c>
       <c r="F170" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-3.0370041690160887E-3</v>
       </c>
       <c r="G170">
@@ -13668,7 +13780,7 @@
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>0.15119333777777777</v>
       </c>
-      <c r="M170" s="35">
+      <c r="M170" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>-0.63835290439629366</v>
       </c>
@@ -13691,7 +13803,7 @@
         <v>20</v>
       </c>
       <c r="F171" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4.4646091210487349E-4</v>
       </c>
       <c r="G171">
@@ -13714,7 +13826,7 @@
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>0.2362752127777778</v>
       </c>
-      <c r="M171" s="35">
+      <c r="M171" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>0.59573601867790682</v>
       </c>
@@ -13737,7 +13849,7 @@
         <v>20</v>
       </c>
       <c r="F172" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-1.1978634981496539E-3</v>
       </c>
       <c r="G172">
@@ -13760,7 +13872,7 @@
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>0.36892216194444449</v>
       </c>
-      <c r="M172" s="35">
+      <c r="M172" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>-8.95655726674571E-2</v>
       </c>
@@ -13798,15 +13910,15 @@
       <c r="J173">
         <v>1.0073848700000001</v>
       </c>
-      <c r="K173" s="34">
+      <c r="K173">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>69.577252268025219</v>
       </c>
-      <c r="L173" s="34">
+      <c r="L173">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>0.55893108194444441</v>
       </c>
-      <c r="M173" s="35">
+      <c r="M173" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>5.7037756018169336E-2</v>
       </c>
@@ -13844,15 +13956,15 @@
       <c r="J174">
         <v>1.1258256600000001</v>
       </c>
-      <c r="K174" s="34">
+      <c r="K174">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>70.316398951619576</v>
       </c>
-      <c r="L174" s="34">
+      <c r="L174">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>0.63206371638888892</v>
       </c>
-      <c r="M174" s="35">
+      <c r="M174" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>0.73255339952120957</v>
       </c>
@@ -13890,15 +14002,15 @@
       <c r="J175">
         <v>1.0900376899999999</v>
       </c>
-      <c r="K175" s="34">
+      <c r="K175">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>71.391841289451264</v>
       </c>
-      <c r="L175" s="34">
+      <c r="L175">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>0.70036014055555562</v>
       </c>
-      <c r="M175" s="35">
+      <c r="M175" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>1.262593084648296</v>
       </c>
@@ -13921,7 +14033,7 @@
         <v>20</v>
       </c>
       <c r="F176" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2393580262437531E-4</v>
       </c>
       <c r="G176">
@@ -13944,7 +14056,7 @@
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>0.73493317555555548</v>
       </c>
-      <c r="M176" s="35">
+      <c r="M176" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>0.82401370875235602</v>
       </c>
@@ -13967,7 +14079,7 @@
         <v>20</v>
       </c>
       <c r="F177" s="21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-1.9511211545968354E-3</v>
       </c>
       <c r="G177">
@@ -13990,7 +14102,7 @@
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>1.5902536119444444</v>
       </c>
-      <c r="M177" s="35">
+      <c r="M177" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>-0.9204262999349071</v>
       </c>
@@ -14028,15 +14140,15 @@
       <c r="J178">
         <v>1.0944703200000001</v>
       </c>
-      <c r="K178" s="34">
+      <c r="K178">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>66.573780368903982</v>
       </c>
-      <c r="L178" s="34">
+      <c r="L178">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>2.503488096111111</v>
       </c>
-      <c r="M178" s="35">
+      <c r="M178" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>1.9496480697505736</v>
       </c>
@@ -14074,15 +14186,15 @@
       <c r="J179">
         <v>1.0623627899999999</v>
       </c>
-      <c r="K179" s="34">
+      <c r="K179">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>68.646377180287928</v>
       </c>
-      <c r="L179" s="34">
+      <c r="L179">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>3.2372024766666669</v>
       </c>
-      <c r="M179" s="35">
+      <c r="M179" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>0.60310471606181504</v>
       </c>
@@ -14105,7 +14217,7 @@
         <v>20</v>
       </c>
       <c r="F180" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-3.1323702352219485E-3</v>
       </c>
       <c r="G180">
@@ -14166,15 +14278,15 @@
       <c r="J181">
         <v>1.03821366</v>
       </c>
-      <c r="K181" s="34">
+      <c r="K181">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>70.003411819284906</v>
       </c>
-      <c r="L181" s="34">
+      <c r="L181">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>4.7616726766666666</v>
       </c>
-      <c r="M181" s="35">
+      <c r="M181" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>0</v>
       </c>
@@ -14212,15 +14324,15 @@
       <c r="J182">
         <v>1.0187743</v>
       </c>
-      <c r="K182" s="34">
+      <c r="K182">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>78.86900283817009</v>
       </c>
-      <c r="L182" s="34">
+      <c r="L182">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>4.9308204097222221</v>
       </c>
-      <c r="M182" s="35">
+      <c r="M182" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>-0.56529112764078482</v>
       </c>
@@ -14258,15 +14370,15 @@
       <c r="J183">
         <v>1.0560619099999999</v>
       </c>
-      <c r="K183" s="34">
+      <c r="K183">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>74.294171233944994</v>
       </c>
-      <c r="L183" s="34">
+      <c r="L183">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>5.9822249452777783</v>
       </c>
-      <c r="M183" s="35">
+      <c r="M183" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>1.2310124792122508</v>
       </c>
@@ -14304,15 +14416,15 @@
       <c r="J184">
         <v>1.0882582700000001</v>
       </c>
-      <c r="K184" s="34">
+      <c r="K184">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>81.754909126161706</v>
       </c>
-      <c r="L184" s="34">
+      <c r="L184">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>6.1158406919444444</v>
       </c>
-      <c r="M184" s="35">
+      <c r="M184" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>0.89797029040104304</v>
       </c>
@@ -14350,15 +14462,15 @@
       <c r="J185">
         <v>1.0869721299999999</v>
       </c>
-      <c r="K185" s="34">
+      <c r="K185">
         <f>Table479[[#This Row],[N]]*Table479[[#This Row],[interation]]/Table479[[#This Row],[time /s]]</f>
         <v>74.699575822160057</v>
       </c>
-      <c r="L185" s="36">
+      <c r="L185" s="5">
         <f>Table479[[#This Row],[time /s]]/3600</f>
         <v>7.4371982630555555</v>
       </c>
-      <c r="M185" s="35">
+      <c r="M185" s="31">
         <f>(Table479[[#This Row],[eff (stochastic)]]-$C$190)/Table479[[#This Row],[std]]</f>
         <v>1.6067891780662018</v>
       </c>
@@ -14393,225 +14505,2627 @@
         <v>-1.0225429040099376E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="5" t="s">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>28</v>
+      </c>
+      <c r="B196" t="s">
+        <v>29</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="D196" t="s">
+        <v>30</v>
+      </c>
+      <c r="E196" t="s">
+        <v>31</v>
+      </c>
+      <c r="H196" s="25" t="e">
+        <f>AVERAGE(H200:H210)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I196" t="s">
+        <v>49</v>
+      </c>
+      <c r="K196" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E197" t="s">
+        <v>47</v>
+      </c>
+      <c r="F197">
+        <v>20</v>
+      </c>
+      <c r="H197" s="25" t="e">
+        <f>_xlfn.STDEV.S(H200:H210)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>6</v>
+      </c>
+      <c r="B199" t="s">
+        <v>9</v>
+      </c>
+      <c r="C199" t="s">
+        <v>27</v>
+      </c>
+      <c r="D199" t="s">
+        <v>12</v>
+      </c>
+      <c r="E199" t="s">
+        <v>48</v>
+      </c>
+      <c r="F199" t="s">
+        <v>8</v>
+      </c>
+      <c r="G199" t="s">
+        <v>21</v>
+      </c>
+      <c r="H199" t="s">
+        <v>45</v>
+      </c>
+      <c r="I199" t="s">
+        <v>43</v>
+      </c>
+      <c r="J199" t="s">
+        <v>50</v>
+      </c>
+      <c r="K199" t="s">
+        <v>46</v>
+      </c>
+      <c r="L199" t="s">
+        <v>37</v>
+      </c>
+      <c r="M199" t="s">
+        <v>59</v>
+      </c>
+      <c r="N199" t="s">
+        <v>60</v>
+      </c>
+      <c r="O199" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>10</v>
+      </c>
+      <c r="B200" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C200" s="1">
+        <v>0.99778151056273101</v>
+      </c>
+      <c r="D200" s="15"/>
+      <c r="E200">
+        <v>20</v>
+      </c>
+      <c r="F200" s="9">
+        <f>B200/B$5-1</f>
+        <v>-0.98973583836189083</v>
+      </c>
+      <c r="G200" s="3">
+        <v>2.5278640565088999</v>
+      </c>
+      <c r="H200" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I200" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J200" s="30">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-0.96540921447145112</v>
+      </c>
+      <c r="K200" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L200" t="e">
+        <f>K200*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M200" s="14" t="e">
+        <f>K200-L200</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N200" s="14" t="e">
+        <f>K200+L200</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O200" s="21">
+        <f>$C$190</f>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>20</v>
+      </c>
+      <c r="B201" s="1">
+        <v>0.99604425274276098</v>
+      </c>
+      <c r="C201" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D201" s="15"/>
+      <c r="E201">
+        <v>20</v>
+      </c>
+      <c r="F201" s="21">
+        <f>B201/B$5-1</f>
+        <v>2.235592088613747E-2</v>
+      </c>
+      <c r="G201" s="3">
+        <v>1.8378407328742301</v>
+      </c>
+      <c r="H201" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I201" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J201" s="30">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>2.2776788416256966</v>
+      </c>
+      <c r="K201" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L201" t="e">
+        <f>K201*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M201" s="14" t="e">
+        <f t="shared" ref="M201:M222" si="19">K201-L201</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N201" s="14" t="e">
+        <f t="shared" ref="N201:N222" si="20">K201+L201</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O201" s="21">
+        <f t="shared" ref="O201:O222" si="21">$C$190</f>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>50</v>
+      </c>
+      <c r="B202" s="1">
+        <v>0.97999999835377805</v>
+      </c>
+      <c r="C202" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D202" s="15"/>
+      <c r="E202" s="15">
+        <v>20</v>
+      </c>
+      <c r="F202" s="21">
+        <f>B202/B$5-1</f>
+        <v>5.8878388449912222E-3</v>
+      </c>
+      <c r="G202" s="3">
+        <v>2.0000000044527302</v>
+      </c>
+      <c r="H202" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I202" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J202" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>0.67325340272740286</v>
+      </c>
+      <c r="K202" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L202" t="e">
+        <f>K202*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M202" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N202" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O202" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>100</v>
+      </c>
+      <c r="B203" s="1">
+        <v>0.96101446887658604</v>
+      </c>
+      <c r="C203" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D203" s="15"/>
+      <c r="E203" s="15">
+        <v>20</v>
+      </c>
+      <c r="F203" s="23">
+        <f>B203/B$5-1</f>
+        <v>-1.3599215488907412E-2</v>
+      </c>
+      <c r="G203" s="3">
+        <v>1.67878707969189</v>
+      </c>
+      <c r="H203" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I203" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J203" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-1.2252995449917981</v>
+      </c>
+      <c r="K203" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L203" t="e">
+        <f>K203*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M203" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N203" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O203" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>200</v>
+      </c>
+      <c r="B204" s="1">
+        <v>0.98381688494387798</v>
+      </c>
+      <c r="C204" s="1">
+        <v>7.8526443679022197E-3</v>
+      </c>
+      <c r="D204" s="15"/>
+      <c r="E204" s="15">
+        <v>20</v>
+      </c>
+      <c r="F204" s="21">
+        <f>B204/B$5-1</f>
+        <v>9.8055529365028704E-3</v>
+      </c>
+      <c r="G204" s="3">
+        <v>1.70820393517531</v>
+      </c>
+      <c r="H204" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I204" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J204" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>1.3434226896222179</v>
+      </c>
+      <c r="K204" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L204" t="e">
+        <f>K204*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M204" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N204" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O204" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>500</v>
+      </c>
+      <c r="B205" s="1">
+        <v>0.96842317374154796</v>
+      </c>
+      <c r="C205" s="1">
+        <v>6.5933445012788796E-3</v>
+      </c>
+      <c r="D205" s="15"/>
+      <c r="E205" s="15">
+        <v>20</v>
+      </c>
+      <c r="F205" s="21">
+        <f>B205/B$5-1</f>
+        <v>-5.994801062605859E-3</v>
+      </c>
+      <c r="G205" s="3">
+        <v>1.23606797759594</v>
+      </c>
+      <c r="H205" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I205" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J205" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-0.73472432450881842</v>
+      </c>
+      <c r="K205" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L205" t="e">
+        <f>K205*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M205" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N205" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O205" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>800</v>
+      </c>
+      <c r="B206" s="1">
+        <v>0.98123697716501601</v>
+      </c>
+      <c r="C206" s="1">
+        <v>3.9772500991747898E-3</v>
+      </c>
+      <c r="D206" s="15"/>
+      <c r="E206" s="15">
+        <v>20</v>
+      </c>
+      <c r="F206" s="21">
+        <f>B206/B$5-1</f>
+        <v>7.1574938911374009E-3</v>
+      </c>
+      <c r="G206" s="3">
+        <v>1.11529493707889</v>
+      </c>
+      <c r="H206" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I206" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J206" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>2.0037746281445892</v>
+      </c>
+      <c r="K206" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L206" t="e">
+        <f>K206*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M206" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N206" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O206" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>1000</v>
+      </c>
+      <c r="B207" s="1">
+        <v>0.98039252553870804</v>
+      </c>
+      <c r="C207" s="1">
+        <v>3.6593683388320098E-3</v>
+      </c>
+      <c r="D207" s="15"/>
+      <c r="E207" s="15">
+        <v>20</v>
+      </c>
+      <c r="F207" s="23">
+        <f>B207/B$5-1</f>
+        <v>6.290735092338462E-3</v>
+      </c>
+      <c r="G207" s="3">
+        <v>1.6261646097200499</v>
+      </c>
+      <c r="H207" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I207" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J207" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>1.9470740719361921</v>
+      </c>
+      <c r="K207" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L207" t="e">
+        <f>K207*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M207" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N207" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O207" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>2000</v>
+      </c>
+      <c r="B208" s="1">
+        <v>0.97899261247595903</v>
+      </c>
+      <c r="C208" s="1">
+        <v>2.7098229053903302E-3</v>
+      </c>
+      <c r="D208" s="15"/>
+      <c r="E208" s="15">
+        <v>20</v>
+      </c>
+      <c r="F208" s="23">
+        <f>B208/B$5-1</f>
+        <v>4.8538416968029185E-3</v>
+      </c>
+      <c r="G208" s="3">
+        <v>1.61803399102434</v>
+      </c>
+      <c r="H208" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I208" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J208" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>2.1127388576082433</v>
+      </c>
+      <c r="K208" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L208" t="e">
+        <f>K208*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M208" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N208" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O208" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>3000</v>
+      </c>
+      <c r="B209" s="1">
+        <v>0.97554422742768399</v>
+      </c>
+      <c r="C209" s="1">
+        <v>2.36329016122537E-3</v>
+      </c>
+      <c r="D209" s="15"/>
+      <c r="E209" s="15">
+        <v>20</v>
+      </c>
+      <c r="F209" s="23">
+        <f>B209/B$5-1</f>
+        <v>1.3143635442094403E-3</v>
+      </c>
+      <c r="G209" s="3">
+        <v>1</v>
+      </c>
+      <c r="H209" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I209" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J209" s="34">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>0.96338703496292755</v>
+      </c>
+      <c r="K209" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L209" t="e">
+        <f>K209*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M209" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N209" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O209" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>5000</v>
+      </c>
+      <c r="B210" s="1">
+        <v>0.97142605865169895</v>
+      </c>
+      <c r="C210" s="1">
+        <v>2.00369256336264E-3</v>
+      </c>
+      <c r="D210" s="15"/>
+      <c r="E210" s="15">
+        <v>20</v>
+      </c>
+      <c r="F210" s="23">
+        <f>B210/B$5-1</f>
+        <v>-2.9125914527630137E-3</v>
+      </c>
+      <c r="G210" s="3">
+        <v>1.0130486540650101</v>
+      </c>
+      <c r="H210" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I210" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J210" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-0.91900609328747351</v>
+      </c>
+      <c r="K210" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L210" t="e">
+        <f>K210*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M210" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N210" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O210" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>7000</v>
+      </c>
+      <c r="B211" s="1">
+        <v>0.97147549422273705</v>
+      </c>
+      <c r="C211" s="1">
+        <v>1.6303606546548401E-3</v>
+      </c>
+      <c r="D211" s="15"/>
+      <c r="E211" s="15">
+        <v>20</v>
+      </c>
+      <c r="F211" s="21">
+        <f>B211/B$5-1</f>
+        <v>-2.8618499835822986E-3</v>
+      </c>
+      <c r="G211" s="3">
+        <v>0.94427191054632198</v>
+      </c>
+      <c r="H211" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I211" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J211" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-1.0991249688531921</v>
+      </c>
+      <c r="K211" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L211" t="e">
+        <f>K211*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M211" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N211" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O211" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>8000</v>
+      </c>
+      <c r="B212" s="1">
+        <v>0.97163373175414403</v>
+      </c>
+      <c r="C212" s="1">
+        <v>1.5695898843485401E-3</v>
+      </c>
+      <c r="D212" s="15"/>
+      <c r="E212" s="15">
+        <v>20</v>
+      </c>
+      <c r="F212" s="21">
+        <f>B212/B$5-1</f>
+        <v>-2.6994324236246925E-3</v>
+      </c>
+      <c r="G212" s="3">
+        <v>1.0062112399500101</v>
+      </c>
+      <c r="H212" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I212" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J212" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-1.0408658902883245</v>
+      </c>
+      <c r="K212" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L212" t="e">
+        <f>K212*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M212" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N212" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O212" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>9000</v>
+      </c>
+      <c r="B213" s="1">
+        <v>0.97045839649051802</v>
+      </c>
+      <c r="C213" s="1">
+        <v>1.5003346884566E-3</v>
+      </c>
+      <c r="D213" s="15"/>
+      <c r="E213" s="15">
+        <v>20</v>
+      </c>
+      <c r="F213" s="21">
+        <f>B213/B$5-1</f>
+        <v>-3.9058155361073599E-3</v>
+      </c>
+      <c r="G213" s="3">
+        <v>1</v>
+      </c>
+      <c r="H213" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I213" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J213" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-1.8722941338346979</v>
+      </c>
+      <c r="K213" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L213" t="e">
+        <f>K213*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M213" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N213" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O213" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A214">
+        <v>10000</v>
+      </c>
+      <c r="B214" s="1">
+        <v>0.97550100952841601</v>
+      </c>
+      <c r="C214" s="1">
+        <v>1.3045292308946901E-3</v>
+      </c>
+      <c r="D214" s="15"/>
+      <c r="E214" s="15">
+        <v>17</v>
+      </c>
+      <c r="F214" s="23">
+        <f>B214/B$5-1</f>
+        <v>1.2700039938349228E-3</v>
+      </c>
+      <c r="G214" s="3">
+        <v>1.13968679345817</v>
+      </c>
+      <c r="H214" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I214" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J214" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>1.7121465345626252</v>
+      </c>
+      <c r="K214" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L214" t="e">
+        <f>K214*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M214" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N214" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O214" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A215">
+        <v>20000</v>
+      </c>
+      <c r="B215" s="1">
+        <v>0.97366738058981706</v>
+      </c>
+      <c r="C215" s="1">
+        <v>9.6926193914101801E-4</v>
+      </c>
+      <c r="D215" s="15"/>
+      <c r="E215" s="15">
+        <v>20</v>
+      </c>
+      <c r="F215" s="21">
+        <f>B215/B$5-1</f>
+        <v>-6.1206238717459449E-4</v>
+      </c>
+      <c r="G215" s="3">
+        <v>1.0770143261184699</v>
+      </c>
+      <c r="H215" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I215" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J215" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>0.41259874876285052</v>
+      </c>
+      <c r="K215" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L215" t="e">
+        <f>K215*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M215" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N215" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O215" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A216">
+        <v>30000</v>
+      </c>
+      <c r="B216" s="1">
+        <v>0.97302916245732296</v>
+      </c>
+      <c r="C216" s="1">
+        <v>7.9224219322948295E-4</v>
+      </c>
+      <c r="D216" s="15"/>
+      <c r="E216" s="15">
+        <v>20</v>
+      </c>
+      <c r="F216" s="21">
+        <f>B216/B$5-1</f>
+        <v>-1.2671397944037377E-3</v>
+      </c>
+      <c r="G216" s="3">
+        <v>1.0475974712581599</v>
+      </c>
+      <c r="H216" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I216" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J216" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-0.30079421573047882</v>
+      </c>
+      <c r="K216" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L216" t="e">
+        <f>K216*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M216" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N216" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O216" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>40000</v>
+      </c>
+      <c r="B217" s="1">
+        <v>0.97173194120821604</v>
+      </c>
+      <c r="C217" s="1">
+        <v>7.10473958237109E-4</v>
+      </c>
+      <c r="D217" s="15"/>
+      <c r="E217" s="15">
+        <v>20</v>
+      </c>
+      <c r="F217" s="21">
+        <f>B217/B$5-1</f>
+        <v>-2.5986286525260249E-3</v>
+      </c>
+      <c r="G217" s="3">
+        <v>1.03444185353721</v>
+      </c>
+      <c r="H217" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I217" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J217" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-2.161265871163033</v>
+      </c>
+      <c r="K217" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L217" t="e">
+        <f>K217*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M217" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N217" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O217" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>60000</v>
+      </c>
+      <c r="B218" s="1">
+        <v>0.97386592139766803</v>
+      </c>
+      <c r="C218" s="1">
+        <v>5.6050154178285201E-4</v>
+      </c>
+      <c r="D218" s="15"/>
+      <c r="E218" s="15">
+        <v>20</v>
+      </c>
+      <c r="F218" s="21">
+        <f>B218/B$5-1</f>
+        <v>-4.0827689282030288E-4</v>
+      </c>
+      <c r="G218" s="3">
+        <v>1.08943680606933</v>
+      </c>
+      <c r="H218" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I218" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J218" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>1.0677170829190483</v>
+      </c>
+      <c r="K218" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L218" t="e">
+        <f>K218*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M218" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N218" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O218" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>70000</v>
+      </c>
+      <c r="B219" s="1">
+        <v>0.97254630290233501</v>
+      </c>
+      <c r="C219" s="1">
+        <v>5.3113888234301897E-4</v>
+      </c>
+      <c r="D219" s="15"/>
+      <c r="E219" s="15">
+        <v>20</v>
+      </c>
+      <c r="F219" s="21">
+        <f>B219/B$5-1</f>
+        <v>-1.7627546464938915E-3</v>
+      </c>
+      <c r="G219" s="3">
+        <v>1.0770143260222</v>
+      </c>
+      <c r="H219" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I219" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J219" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-1.3577643214289563</v>
+      </c>
+      <c r="K219" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L219" t="e">
+        <f>K219*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M219" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N219" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O219" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>80000</v>
+      </c>
+      <c r="B220" s="1">
+        <v>0.97282099917831999</v>
+      </c>
+      <c r="C220" s="1">
+        <v>4.9469940309467095E-4</v>
+      </c>
+      <c r="D220" s="15"/>
+      <c r="E220" s="15">
+        <v>20</v>
+      </c>
+      <c r="F220" s="21">
+        <f>B220/B$5-1</f>
+        <v>-1.4808019486842738E-3</v>
+      </c>
+      <c r="G220" s="3">
+        <v>1.0425724724849801</v>
+      </c>
+      <c r="H220" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I220" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J220" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-0.90249785100021085</v>
+      </c>
+      <c r="K220" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L220" t="e">
+        <f>K220*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M220" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N220" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O220" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>90000</v>
+      </c>
+      <c r="B221" s="1">
+        <v>0.97247964813441801</v>
+      </c>
+      <c r="C221" s="1">
+        <v>4.7184712979378402E-4</v>
+      </c>
+      <c r="D221" s="15"/>
+      <c r="E221" s="15">
+        <v>20</v>
+      </c>
+      <c r="F221" s="21">
+        <f>B221/B$5-1</f>
+        <v>-1.8311701776789757E-3</v>
+      </c>
+      <c r="G221" s="3">
+        <v>1.0433056099716</v>
+      </c>
+      <c r="H221" s="15" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I221" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J221" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-1.6696428617258254</v>
+      </c>
+      <c r="K221" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L221" t="e">
+        <f>K221*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M221" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N221" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O221" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>100000</v>
+      </c>
+      <c r="B222" s="1">
+        <v>0.972742820219895</v>
+      </c>
+      <c r="C222" s="1">
+        <v>4.4602393481509402E-4</v>
+      </c>
+      <c r="D222" s="15"/>
+      <c r="E222" s="15">
+        <v>20</v>
+      </c>
+      <c r="F222" s="21">
+        <f>B222/B$5-1</f>
+        <v>-1.5610460952816263E-3</v>
+      </c>
+      <c r="G222">
+        <v>1.0557280899538699</v>
+      </c>
+      <c r="H222" t="e">
+        <f>Table4810[[#This Row],[N]]*Table4810[[#This Row],[interation]]/Table4810[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I222" s="25">
+        <f>Table4810[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="J222" s="31">
+        <f>(Table4810[[#This Row],[eff (stochastic)]]-$C$190)/Table4810[[#This Row],[std]]</f>
+        <v>-1.1762689525317001</v>
+      </c>
+      <c r="K222" s="14" t="str">
+        <f>D$5</f>
+        <v>eff (anaytical)</v>
+      </c>
+      <c r="L222" t="e">
+        <f>K222*K$3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M222" s="14" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N222" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O222" s="21">
+        <f t="shared" si="21"/>
+        <v>0.97326746432650402</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>28</v>
+      </c>
+      <c r="B225" t="s">
+        <v>29</v>
+      </c>
+      <c r="C225">
+        <v>1</v>
+      </c>
+      <c r="D225" t="s">
+        <v>30</v>
+      </c>
+      <c r="E225" t="s">
+        <v>33</v>
+      </c>
+      <c r="H225" s="25" t="e">
+        <f>AVERAGE(K229:K239)*3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I225" t="s">
+        <v>49</v>
+      </c>
+      <c r="K225" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E226" t="s">
+        <v>47</v>
+      </c>
+      <c r="F226">
+        <v>20</v>
+      </c>
+      <c r="H226" s="25" t="e">
+        <f>_xlfn.STDEV.S(K229:K239)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>6</v>
+      </c>
+      <c r="B228" t="s">
+        <v>9</v>
+      </c>
+      <c r="C228" t="s">
+        <v>27</v>
+      </c>
+      <c r="D228" t="s">
+        <v>12</v>
+      </c>
+      <c r="E228" t="s">
+        <v>48</v>
+      </c>
+      <c r="F228" t="s">
+        <v>8</v>
+      </c>
+      <c r="G228" t="s">
+        <v>21</v>
+      </c>
+      <c r="H228" t="s">
+        <v>22</v>
+      </c>
+      <c r="I228" t="s">
+        <v>23</v>
+      </c>
+      <c r="J228" t="s">
+        <v>24</v>
+      </c>
+      <c r="K228" t="s">
+        <v>45</v>
+      </c>
+      <c r="L228" t="s">
+        <v>43</v>
+      </c>
+      <c r="M228" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A229">
+        <v>10</v>
+      </c>
+      <c r="B229" s="1">
+        <v>0.93450916376549398</v>
+      </c>
+      <c r="C229" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D229" s="15"/>
+      <c r="E229">
+        <v>20</v>
+      </c>
+      <c r="F229" s="9">
+        <f t="shared" ref="F229:F239" si="22">B229/B$5-1</f>
+        <v>-4.0804689081672452E-2</v>
+      </c>
+      <c r="G229">
+        <v>4.0368364330743303</v>
+      </c>
+      <c r="H229">
+        <v>4.0986145499999997</v>
+      </c>
+      <c r="I229">
+        <v>4.0874667699999998</v>
+      </c>
+      <c r="J229">
+        <v>3.9244279799999999</v>
+      </c>
+      <c r="K229" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L229">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M229" s="30">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-3.875830056101004</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>20</v>
+      </c>
+      <c r="B230" s="1">
+        <v>0.97869541156450501</v>
+      </c>
+      <c r="C230" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D230" s="15"/>
+      <c r="E230">
+        <v>20</v>
+      </c>
+      <c r="F230" s="21">
+        <f t="shared" si="22"/>
+        <v>4.5487898773870494E-3</v>
+      </c>
+      <c r="G230">
+        <v>2.9018462997320902</v>
+      </c>
+      <c r="H230">
+        <v>3.0445600499999999</v>
+      </c>
+      <c r="I230">
+        <v>2.87806067</v>
+      </c>
+      <c r="J230">
+        <v>2.7829181699999999</v>
+      </c>
+      <c r="K230" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L230">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M230" s="30">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>0.54279472380009963</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>50</v>
+      </c>
+      <c r="B231" s="1">
+        <v>0.93816997184992801</v>
+      </c>
+      <c r="C231" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D231" s="15"/>
+      <c r="E231" s="15">
+        <v>20</v>
+      </c>
+      <c r="F231" s="21">
+        <f t="shared" si="22"/>
+        <v>-3.7047176491199707E-2</v>
+      </c>
+      <c r="G231">
+        <v>1.0165979456018499</v>
+      </c>
+      <c r="H231">
+        <v>1.0246853300000001</v>
+      </c>
+      <c r="I231">
+        <v>1.00007595</v>
+      </c>
+      <c r="J231">
+        <v>1.0250325499999999</v>
+      </c>
+      <c r="K231" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L231">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M231" s="30">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-3.5097492476576009</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>100</v>
+      </c>
+      <c r="B232" s="1">
+        <v>0.97289296112007895</v>
+      </c>
+      <c r="C232" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D232" s="15"/>
+      <c r="E232" s="15">
+        <v>20</v>
+      </c>
+      <c r="F232" s="23">
+        <f t="shared" si="22"/>
+        <v>-1.4069390484836575E-3</v>
+      </c>
+      <c r="G232">
+        <v>1.0074074074074</v>
+      </c>
+      <c r="H232">
+        <v>1.03703704</v>
+      </c>
+      <c r="I232">
+        <v>1.03703704</v>
+      </c>
+      <c r="J232">
+        <v>0.94814814999999997</v>
+      </c>
+      <c r="K232" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L232">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M232" s="30">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-3.7450320642506973E-2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>200</v>
+      </c>
+      <c r="B233" s="1">
+        <v>0.97543719781386695</v>
+      </c>
+      <c r="C233" s="1">
+        <v>9.8395618072187503E-3</v>
+      </c>
+      <c r="D233" s="15"/>
+      <c r="E233" s="15">
+        <v>20</v>
+      </c>
+      <c r="F233" s="21">
+        <f t="shared" si="22"/>
+        <v>1.2045066185812914E-3</v>
+      </c>
+      <c r="G233">
+        <v>1.39415607225691</v>
+      </c>
+      <c r="H233">
+        <v>1.36378625</v>
+      </c>
+      <c r="I233">
+        <v>1.43832457</v>
+      </c>
+      <c r="J233">
+        <v>1.3803574000000001</v>
+      </c>
+      <c r="K233" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L233">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M233" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>0.22051119042426459</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>500</v>
+      </c>
+      <c r="B234" s="1">
+        <v>0.97029361394063696</v>
+      </c>
+      <c r="C234" s="1">
+        <v>6.4093961290366897E-3</v>
+      </c>
+      <c r="D234" s="15"/>
+      <c r="E234" s="15">
+        <v>20</v>
+      </c>
+      <c r="F234" s="21">
+        <f t="shared" si="22"/>
+        <v>-4.074951008819272E-3</v>
+      </c>
+      <c r="G234">
+        <v>1.00236395031238</v>
+      </c>
+      <c r="H234">
+        <v>1.0002800300000001</v>
+      </c>
+      <c r="I234">
+        <v>1.00653178</v>
+      </c>
+      <c r="J234">
+        <v>1.0002800300000001</v>
+      </c>
+      <c r="K234" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L234">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M234" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-0.46398292850000833</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>800</v>
+      </c>
+      <c r="B235" s="1">
+        <v>0.97468823329890497</v>
+      </c>
+      <c r="C235" s="1">
+        <v>4.6233842384465996E-3</v>
+      </c>
+      <c r="D235" s="15"/>
+      <c r="E235" s="15">
+        <v>20</v>
+      </c>
+      <c r="F235" s="21">
+        <f t="shared" si="22"/>
+        <v>4.3575733430345487E-4</v>
+      </c>
+      <c r="G235">
+        <v>1.10316348515197</v>
+      </c>
+      <c r="H235">
+        <v>1.08507884</v>
+      </c>
+      <c r="I235">
+        <v>1.1393327799999999</v>
+      </c>
+      <c r="J235">
+        <v>1.08507884</v>
+      </c>
+      <c r="K235" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L235">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M235" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>0.30730064799423101</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>1000</v>
+      </c>
+      <c r="B236" s="1">
+        <v>0.97891659343794302</v>
+      </c>
+      <c r="C236" s="1">
+        <v>4.0099214797694903E-3</v>
+      </c>
+      <c r="D236" s="15"/>
+      <c r="E236" s="15">
+        <v>20</v>
+      </c>
+      <c r="F236" s="23">
+        <f t="shared" si="22"/>
+        <v>4.7758145274259256E-3</v>
+      </c>
+      <c r="G236">
+        <v>1.1133123301401999</v>
+      </c>
+      <c r="H236">
+        <v>1.1145179000000001</v>
+      </c>
+      <c r="I236">
+        <v>1.13296949</v>
+      </c>
+      <c r="J236">
+        <v>1.0924495999999999</v>
+      </c>
+      <c r="K236" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L236">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M236" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>1.4087879625422837</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>2000</v>
+      </c>
+      <c r="B237" s="1">
+        <v>0.96754814632254404</v>
+      </c>
+      <c r="C237" s="1">
+        <v>3.3564970231109801E-3</v>
+      </c>
+      <c r="D237" s="15"/>
+      <c r="E237" s="15">
+        <v>20</v>
+      </c>
+      <c r="F237" s="23">
+        <f t="shared" si="22"/>
+        <v>-6.8929433492492809E-3</v>
+      </c>
+      <c r="G237">
+        <v>0.92873605472418796</v>
+      </c>
+      <c r="H237">
+        <v>0.91709686000000001</v>
+      </c>
+      <c r="I237">
+        <v>0.95102695999999998</v>
+      </c>
+      <c r="J237">
+        <v>0.91808434999999999</v>
+      </c>
+      <c r="K237" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L237">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M237" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-1.7039544395779038</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>3000</v>
+      </c>
+      <c r="B238" s="1">
+        <v>0.97267008325387505</v>
+      </c>
+      <c r="C238" s="1">
+        <v>2.51907446833882E-3</v>
+      </c>
+      <c r="D238" s="15"/>
+      <c r="E238" s="15">
+        <v>20</v>
+      </c>
+      <c r="F238" s="23">
+        <f t="shared" si="22"/>
+        <v>-1.6357044929110609E-3</v>
+      </c>
+      <c r="G238">
+        <v>1.0084005377335501</v>
+      </c>
+      <c r="H238">
+        <v>1.0414628500000001</v>
+      </c>
+      <c r="I238">
+        <v>0.99186938000000002</v>
+      </c>
+      <c r="J238">
+        <v>0.99186938000000002</v>
+      </c>
+      <c r="K238" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L238">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M238" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-0.23714307779988086</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>5000</v>
+      </c>
+      <c r="B239" s="1">
+        <v>0.97160071871703002</v>
+      </c>
+      <c r="C239" s="1">
+        <v>1.9544728371047901E-3</v>
+      </c>
+      <c r="D239" s="15"/>
+      <c r="E239" s="15">
+        <v>20</v>
+      </c>
+      <c r="F239" s="23">
+        <f t="shared" si="22"/>
+        <v>-2.7333175385348962E-3</v>
+      </c>
+      <c r="G239">
+        <v>0.94865499547389498</v>
+      </c>
+      <c r="H239">
+        <v>0.93843957</v>
+      </c>
+      <c r="I239">
+        <v>0.95209728000000005</v>
+      </c>
+      <c r="J239">
+        <v>0.95542813999999998</v>
+      </c>
+      <c r="K239" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L239">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M239" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-0.85278525126140337</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>7000</v>
+      </c>
+      <c r="B240" s="1">
+        <v>0.97612852099638903</v>
+      </c>
+      <c r="C240" s="1">
+        <v>1.52240246336817E-3</v>
+      </c>
+      <c r="D240" s="15"/>
+      <c r="E240" s="15">
+        <v>20</v>
+      </c>
+      <c r="F240" s="21">
+        <f>B240/B$5-1</f>
+        <v>1.9140919075391061E-3</v>
+      </c>
+      <c r="G240">
+        <v>1.0784913888436201</v>
+      </c>
+      <c r="H240">
+        <v>1.0641694799999999</v>
+      </c>
+      <c r="I240">
+        <v>1.1056443</v>
+      </c>
+      <c r="J240">
+        <v>1.0656603899999999</v>
+      </c>
+      <c r="K240" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L240">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M240" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>1.8793037575328109</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>8000</v>
+      </c>
+      <c r="B241" s="1">
+        <v>0.97462985071487296</v>
+      </c>
+      <c r="C241" s="1">
+        <v>1.47780303234547E-3</v>
+      </c>
+      <c r="D241" s="15"/>
+      <c r="E241" s="15">
+        <v>20</v>
+      </c>
+      <c r="F241" s="21">
+        <f>B241/B$5-1</f>
+        <v>3.7583250636785692E-4</v>
+      </c>
+      <c r="G241">
+        <v>1.0878918523082799</v>
+      </c>
+      <c r="H241">
+        <v>1.07403223</v>
+      </c>
+      <c r="I241">
+        <v>1.1127658600000001</v>
+      </c>
+      <c r="J241">
+        <v>1.07687746</v>
+      </c>
+      <c r="K241" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L241">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M241" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>0.92189984629186539</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>9000</v>
+      </c>
+      <c r="B242" s="1">
+        <v>0.97439023942940295</v>
+      </c>
+      <c r="C242" s="1">
+        <v>1.3981512838358099E-3</v>
+      </c>
+      <c r="D242" s="15"/>
+      <c r="E242" s="15">
+        <v>20</v>
+      </c>
+      <c r="F242" s="21">
+        <f>B242/B$5-1</f>
+        <v>1.2989160992993298E-4</v>
+      </c>
+      <c r="G242">
+        <v>1.0637414407197501</v>
+      </c>
+      <c r="H242">
+        <v>1.05572512</v>
+      </c>
+      <c r="I242">
+        <v>1.08174974</v>
+      </c>
+      <c r="J242">
+        <v>1.0537494599999999</v>
+      </c>
+      <c r="K242" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L242">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M242" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>0.8030426434388509</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>10000</v>
+      </c>
+      <c r="B243" s="1">
+        <v>0.972634040637954</v>
+      </c>
+      <c r="C243" s="1">
+        <v>1.3792076766175E-3</v>
+      </c>
+      <c r="D243" s="15"/>
+      <c r="E243" s="15">
+        <v>20</v>
+      </c>
+      <c r="F243" s="9">
+        <f t="shared" ref="F243:F244" si="23">B243/B$5-1</f>
+        <v>-1.6726992164783905E-3</v>
+      </c>
+      <c r="G243">
+        <v>1.1036447157967699</v>
+      </c>
+      <c r="H243">
+        <v>1.08576563</v>
+      </c>
+      <c r="I243">
+        <v>1.13966926</v>
+      </c>
+      <c r="J243">
+        <v>1.08549926</v>
+      </c>
+      <c r="K243" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L243">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M243" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-0.45926635943869243</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>20000</v>
+      </c>
+      <c r="B244" s="1">
+        <v>0.97378125659533799</v>
+      </c>
+      <c r="C244" s="1">
+        <v>9.6727936931309902E-4</v>
+      </c>
+      <c r="D244" s="15"/>
+      <c r="E244" s="15">
+        <v>20</v>
+      </c>
+      <c r="F244" s="21">
+        <f t="shared" si="23"/>
+        <v>-4.9517821443767485E-4</v>
+      </c>
+      <c r="G244">
+        <v>1.0963796279126701</v>
+      </c>
+      <c r="H244">
+        <v>1.0908777300000001</v>
+      </c>
+      <c r="I244">
+        <v>1.1128291800000001</v>
+      </c>
+      <c r="J244">
+        <v>1.0854319699999999</v>
+      </c>
+      <c r="K244" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L244">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M244" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>0.53117257033904375</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>30000</v>
+      </c>
+      <c r="B245" s="1">
+        <v>0.974199460870523</v>
+      </c>
+      <c r="C245" s="1">
+        <v>7.7669906616381602E-4</v>
+      </c>
+      <c r="D245" s="15"/>
+      <c r="E245" s="15">
+        <v>20</v>
+      </c>
+      <c r="F245" s="21">
+        <f>B245/B$5-1</f>
+        <v>-6.5926586612974347E-5</v>
+      </c>
+      <c r="G245">
+        <v>1.0922866585598101</v>
+      </c>
+      <c r="H245">
+        <v>1.07815846</v>
+      </c>
+      <c r="I245">
+        <v>1.1099469099999999</v>
+      </c>
+      <c r="J245">
+        <v>1.0887546100000001</v>
+      </c>
+      <c r="K245" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L245">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M245" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>1.1999454932039493</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>40000</v>
+      </c>
+      <c r="B246" s="1">
+        <v>0.97234407008623602</v>
+      </c>
+      <c r="C246" s="1">
+        <v>7.0650682818022403E-4</v>
+      </c>
+      <c r="D246" s="15"/>
+      <c r="E246" s="15">
+        <v>20</v>
+      </c>
+      <c r="F246" s="21">
+        <f>B246/B$5-1</f>
+        <v>-1.9703296777908719E-3</v>
+      </c>
+      <c r="G246">
+        <v>1.0549978983847801</v>
+      </c>
+      <c r="H246">
+        <v>1.0480488100000001</v>
+      </c>
+      <c r="I246">
+        <v>1.0733032600000001</v>
+      </c>
+      <c r="J246">
+        <v>1.04364163</v>
+      </c>
+      <c r="K246" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L246">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M246" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-1.3069855851873575</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>60000</v>
+      </c>
+      <c r="B247" s="1">
+        <v>0.97215806362563195</v>
+      </c>
+      <c r="C247" s="24">
+        <v>5.79752614690079E-4</v>
+      </c>
+      <c r="D247" s="15"/>
+      <c r="E247" s="15">
+        <v>20</v>
+      </c>
+      <c r="F247" s="22">
+        <f>B247/B$5-1</f>
+        <v>-2.161249715528224E-3</v>
+      </c>
+      <c r="G247">
+        <v>1.0493053241535</v>
+      </c>
+      <c r="H247">
+        <v>1.04121321</v>
+      </c>
+      <c r="I247">
+        <v>1.06901651</v>
+      </c>
+      <c r="J247">
+        <v>1.0376862499999999</v>
+      </c>
+      <c r="K247" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L247">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M247" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-1.9135760197737488</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>70000</v>
+      </c>
+      <c r="B248" s="1">
+        <v>0.97256866184810697</v>
+      </c>
+      <c r="C248" s="24">
+        <v>5.3117779113690596E-4</v>
+      </c>
+      <c r="D248" s="15"/>
+      <c r="E248" s="15">
+        <v>20</v>
+      </c>
+      <c r="F248" s="22">
+        <f>B248/B$5-1</f>
+        <v>-1.739805063147859E-3</v>
+      </c>
+      <c r="G248">
+        <v>1.04805033853489</v>
+      </c>
+      <c r="H248">
+        <v>1.04420446</v>
+      </c>
+      <c r="I248">
+        <v>1.06857801</v>
+      </c>
+      <c r="J248">
+        <v>1.0313685399999999</v>
+      </c>
+      <c r="K248" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L248">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M248" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-1.3155717163952982</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>80000</v>
+      </c>
+      <c r="B249" s="1">
+        <v>0.97285065629054002</v>
+      </c>
+      <c r="C249" s="24">
+        <v>4.9806844688671801E-4</v>
+      </c>
+      <c r="D249" s="15"/>
+      <c r="E249" s="15">
+        <v>20</v>
+      </c>
+      <c r="F249" s="22">
+        <f>B249/B$5-1</f>
+        <v>-1.4503614093296369E-3</v>
+      </c>
+      <c r="G249">
+        <v>1.0785408377810599</v>
+      </c>
+      <c r="H249">
+        <v>1.0706824800000001</v>
+      </c>
+      <c r="I249">
+        <v>1.10433176</v>
+      </c>
+      <c r="J249">
+        <v>1.0606082800000001</v>
+      </c>
+      <c r="K249" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L249">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M249" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-0.83684890815579049</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>90000</v>
+      </c>
+      <c r="B250" s="1">
+        <v>0.97398483701930805</v>
+      </c>
+      <c r="C250" s="24">
+        <v>4.5871639258491999E-4</v>
+      </c>
+      <c r="D250" s="15"/>
+      <c r="E250" s="15">
+        <v>20</v>
+      </c>
+      <c r="F250" s="22">
+        <f>B250/B$5-1</f>
+        <v>-2.8621997663935694E-4</v>
+      </c>
+      <c r="G250">
+        <v>1.0865785018196701</v>
+      </c>
+      <c r="H250">
+        <v>1.0833461900000001</v>
+      </c>
+      <c r="I250">
+        <v>1.09927054</v>
+      </c>
+      <c r="J250">
+        <v>1.0771187799999999</v>
+      </c>
+      <c r="K250" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L250">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M250" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>1.5638697556927321</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>100000</v>
+      </c>
+      <c r="B251" s="1">
+        <v>0.97261275469606201</v>
+      </c>
+      <c r="C251" s="24">
+        <v>4.4868113413586001E-4</v>
+      </c>
+      <c r="D251" s="15"/>
+      <c r="E251" s="15">
+        <v>20</v>
+      </c>
+      <c r="F251" s="22">
+        <f>B251/B$5-1</f>
+        <v>-1.6945474512982672E-3</v>
+      </c>
+      <c r="G251">
+        <v>1.04068526668376</v>
+      </c>
+      <c r="H251">
+        <v>1.03471326</v>
+      </c>
+      <c r="I251">
+        <v>1.06496455</v>
+      </c>
+      <c r="J251">
+        <v>1.022378</v>
+      </c>
+      <c r="K251" t="e">
+        <f>Table47912[[#This Row],[N]]*Table47912[[#This Row],[interation]]/Table47912[[#This Row],[time /s]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L251" s="5">
+        <f>Table47912[[#This Row],[time /s]]/3600</f>
+        <v>0</v>
+      </c>
+      <c r="M251" s="31">
+        <f>(Table47912[[#This Row],[eff (stochastic)]]-$C$190)/Table47912[[#This Row],[std]]</f>
+        <v>-1.4591868938348593</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A255" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="5" t="s">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A256" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" s="5" t="s">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="5" t="s">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
         <v>57</v>
       </c>
-      <c r="B200">
+      <c r="B261">
         <v>7062</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C201" t="s">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C262" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
         <v>66</v>
       </c>
-      <c r="B202">
+      <c r="B263">
         <v>-12</v>
       </c>
-      <c r="C202" s="14">
-        <f>B202/B$200</f>
+      <c r="C263" s="14">
+        <f>B263/B$261</f>
         <v>-1.6992353440951572E-3</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B203">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B264">
         <v>-23</v>
       </c>
-      <c r="C203" s="14">
-        <f t="shared" ref="C203:C221" si="18">B203/B$200</f>
+      <c r="C264" s="14">
+        <f t="shared" ref="C264:C282" si="24">B264/B$261</f>
         <v>-3.2568677428490515E-3</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B204">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B265">
         <v>39</v>
       </c>
-      <c r="C204" s="14">
-        <f t="shared" si="18"/>
+      <c r="C265" s="14">
+        <f t="shared" si="24"/>
         <v>5.5225148683092605E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B205">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B266">
         <v>-5</v>
       </c>
-      <c r="C205" s="14">
-        <f t="shared" si="18"/>
+      <c r="C266" s="14">
+        <f t="shared" si="24"/>
         <v>-7.0801472670631554E-4</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B206">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B267">
         <v>8</v>
       </c>
-      <c r="C206" s="14">
-        <f t="shared" si="18"/>
+      <c r="C267" s="14">
+        <f t="shared" si="24"/>
         <v>1.1328235627301047E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B207">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B268">
         <v>3</v>
       </c>
-      <c r="C207" s="14">
-        <f t="shared" si="18"/>
+      <c r="C268" s="14">
+        <f t="shared" si="24"/>
         <v>4.248088360237893E-4</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B208">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B269">
         <v>-10</v>
       </c>
-      <c r="C208" s="14">
-        <f t="shared" si="18"/>
+      <c r="C269" s="14">
+        <f t="shared" si="24"/>
         <v>-1.4160294534126311E-3</v>
       </c>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B209">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B270">
         <v>-14</v>
       </c>
-      <c r="C209" s="14">
-        <f t="shared" si="18"/>
+      <c r="C270" s="14">
+        <f t="shared" si="24"/>
         <v>-1.9824412347776836E-3</v>
       </c>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B210">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B271">
         <v>0</v>
       </c>
-      <c r="C210" s="14">
-        <f t="shared" si="18"/>
+      <c r="C271" s="14">
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B211">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B272">
         <v>7</v>
       </c>
-      <c r="C211" s="14">
-        <f t="shared" si="18"/>
+      <c r="C272" s="14">
+        <f t="shared" si="24"/>
         <v>9.9122061738884178E-4</v>
       </c>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B212">
+    <row r="273" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B273">
         <v>0</v>
       </c>
-      <c r="C212" s="14">
-        <f t="shared" si="18"/>
+      <c r="C273" s="14">
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B213">
+    <row r="274" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B274">
         <v>-15</v>
       </c>
-      <c r="C213" s="14">
-        <f t="shared" si="18"/>
+      <c r="C274" s="14">
+        <f t="shared" si="24"/>
         <v>-2.1240441801189465E-3</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B214">
+    <row r="275" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B275">
         <v>-13</v>
       </c>
-      <c r="C214" s="14">
-        <f t="shared" si="18"/>
+      <c r="C275" s="14">
+        <f t="shared" si="24"/>
         <v>-1.8408382894364204E-3</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B215">
+    <row r="276" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B276">
         <v>14</v>
       </c>
-      <c r="C215" s="14">
-        <f t="shared" si="18"/>
+      <c r="C276" s="14">
+        <f t="shared" si="24"/>
         <v>1.9824412347776836E-3</v>
       </c>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B216">
+    <row r="277" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B277">
         <v>8</v>
       </c>
-      <c r="C216" s="14">
-        <f t="shared" si="18"/>
+      <c r="C277" s="14">
+        <f t="shared" si="24"/>
         <v>1.1328235627301047E-3</v>
       </c>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B217">
+    <row r="278" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B278">
         <v>34</v>
       </c>
-      <c r="C217" s="14">
-        <f t="shared" si="18"/>
+      <c r="C278" s="14">
+        <f t="shared" si="24"/>
         <v>4.8145001416029457E-3</v>
       </c>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B218">
+    <row r="279" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B279">
         <v>-4</v>
       </c>
-      <c r="C218" s="14">
-        <f t="shared" si="18"/>
+      <c r="C279" s="14">
+        <f t="shared" si="24"/>
         <v>-5.6641178136505237E-4</v>
       </c>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B219">
+    <row r="280" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B280">
         <v>-4</v>
       </c>
-      <c r="C219" s="14">
-        <f t="shared" si="18"/>
+      <c r="C280" s="14">
+        <f t="shared" si="24"/>
         <v>-5.6641178136505237E-4</v>
       </c>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B220">
+    <row r="281" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B281">
         <v>6</v>
       </c>
-      <c r="C220" s="14">
-        <f t="shared" si="18"/>
+      <c r="C281" s="14">
+        <f t="shared" si="24"/>
         <v>8.4961767204757861E-4</v>
       </c>
     </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B221">
+    <row r="282" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B282">
         <v>0</v>
       </c>
-      <c r="C221" s="14">
-        <f t="shared" si="18"/>
+      <c r="C282" s="14">
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C223" s="14">
-        <f>AVERAGE(C202:C221)</f>
+    <row r="284" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C284" s="14">
+        <f>AVERAGE(C263:C282)</f>
         <v>1.3452279807419997E-4</v>
       </c>
     </row>
@@ -14620,7 +17134,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="8">
+  <tableParts count="10">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -14629,6 +17143,8 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>